<commit_message>
more automation code & prelim results
</commit_message>
<xml_diff>
--- a/SPIN-to-N3/test/run/cmp_times.xlsx
+++ b/SPIN-to-N3/test/run/cmp_times.xlsx
@@ -8,20 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1974E96A-0BF0-644F-A3A6-05A910C9198E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DBD65A-A8DB-5843-BF52-BFF60E7004E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19840" xr2:uid="{94AE5E48-1175-4942-B1A9-4F55D3AD141D}"/>
   </bookViews>
   <sheets>
-    <sheet name="gmark_50-eye" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="gmark" sheetId="2" r:id="rId1"/>
+    <sheet name="lmdb" sheetId="1" r:id="rId2"/>
+    <sheet name="yago" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="gmark_50_eye" localSheetId="0">'gmark_50-eye'!$A$40:$E$79</definedName>
-    <definedName name="gmark_50_eye_forward" localSheetId="0">'gmark_50-eye'!$H$40:$N$79</definedName>
-    <definedName name="gmark_50_nmo" localSheetId="0">'gmark_50-eye'!$Q$40:$T$70</definedName>
+    <definedName name="gmark_50_eye" localSheetId="0">gmark!$A$40:$E$79</definedName>
+    <definedName name="gmark_50_eye_forward" localSheetId="0">gmark!$H$40:$N$79</definedName>
+    <definedName name="gmark_50_nmo" localSheetId="0">gmark!$Q$40:$T$70</definedName>
+    <definedName name="lmdb_eye" localSheetId="1">lmdb!$A$40:$E$43</definedName>
+    <definedName name="lmdb_recsparql_1" localSheetId="1">lmdb!$O$40:$Q$43</definedName>
+    <definedName name="lmdb_spin" localSheetId="1">lmdb!$H$40:$L$43</definedName>
+    <definedName name="yago_eye" localSheetId="2">yago!$A$32:$E$37</definedName>
+    <definedName name="yago_recsparql" localSheetId="2">yago!$O$32:$Q$37</definedName>
+    <definedName name="yago_spin" localSheetId="2">yago!$H$32:$L$37</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +51,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{7BABB170-5717-FA47-B763-2B6AADA1D962}" name="gmark_50-eye" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/gmark_50-eye.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/gmark_50-eye.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -55,7 +62,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{9EF3F591-4452-6D40-94F1-9E08EAAD0030}" name="gmark_50-eye-forward" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/gmark_50-eye-forward.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/gmark_50-eye-forward.csv" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -68,7 +75,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{615E2C0E-A7EF-194F-9F76-E4800C6945BF}" name="gmark_50-nmo" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/gmark_50-nmo.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/gmark_50-nmo.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -77,14 +84,76 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{B55C9681-E85F-7347-9475-C263A669401A}" keepAlive="1" name="Query - gmark_50-eye" description="Connection to the 'gmark_50-eye' query in the workbook." type="5" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{39F583D4-93FF-5146-994C-646A963F913B}" name="lmdb-eye" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-eye.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" xr16:uid="{FC45E0D5-6402-0341-AB3C-FB00067C91DF}" name="lmdb-recsparql" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-recsparql.csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" xr16:uid="{1E6C00C3-C49D-0A41-B42A-D043CA0AB2F5}" name="lmdb-spin" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-spin.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" xr16:uid="{B55C9681-E85F-7347-9475-C263A669401A}" keepAlive="1" name="Query - gmark_50-eye" description="Connection to the 'gmark_50-eye' query in the workbook." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=gmark_50-eye;Extended Properties=&quot;&quot;" command="SELECT * FROM [gmark_50-eye]"/>
+  </connection>
+  <connection id="8" xr16:uid="{8E824083-4B73-C34C-B75C-E4C5FD24E1F4}" name="yago-eye" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-eye.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" xr16:uid="{A383D5A5-B79F-AB49-9812-02B5108CCB77}" name="yago-recsparql" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-recsparql.csv" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="10" xr16:uid="{8BB0FA84-0301-4F41-98FC-E56B4A9EBBD1}" name="yago-spin" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-spin.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="201">
   <si>
     <t>result_file</t>
   </si>
@@ -573,6 +642,120 @@
   </si>
   <si>
     <t>doesn't complete by nmo:</t>
+  </si>
+  <si>
+    <t>lmdb1</t>
+  </si>
+  <si>
+    <t>lmdb_lmdb-lmdb1.n3</t>
+  </si>
+  <si>
+    <t>lmdb2</t>
+  </si>
+  <si>
+    <t>lmdb_lmdb-lmdb2.n3</t>
+  </si>
+  <si>
+    <t>lmdb3</t>
+  </si>
+  <si>
+    <t>lmdb_lmdb-lmdb3.n3</t>
+  </si>
+  <si>
+    <t>lmdb-lmdb1-spin.nt</t>
+  </si>
+  <si>
+    <t>lmdb-lmdb2-spin.nt</t>
+  </si>
+  <si>
+    <t>lmdb-lmdb3-spin.nt</t>
+  </si>
+  <si>
+    <t>spin</t>
+  </si>
+  <si>
+    <t>sin3</t>
+  </si>
+  <si>
+    <t>lmdb-lmdb1-recsparql.txt</t>
+  </si>
+  <si>
+    <t>lmdb-lmdb2-recsparql.txt</t>
+  </si>
+  <si>
+    <t>lmdb-lmdb3-recsparql.txt</t>
+  </si>
+  <si>
+    <t>recsparql</t>
+  </si>
+  <si>
+    <t>load_time</t>
+  </si>
+  <si>
+    <t>yago1</t>
+  </si>
+  <si>
+    <t>yago_yagoFacts-yago1.n3</t>
+  </si>
+  <si>
+    <t>yago2</t>
+  </si>
+  <si>
+    <t>yago_yagoFacts-yago2.n3</t>
+  </si>
+  <si>
+    <t>yago3</t>
+  </si>
+  <si>
+    <t>yago_yagoFacts-yago3.n3</t>
+  </si>
+  <si>
+    <t>yago4</t>
+  </si>
+  <si>
+    <t>yago_yagoFacts-yago4.n3</t>
+  </si>
+  <si>
+    <t>yago5</t>
+  </si>
+  <si>
+    <t>yago_yagoFacts-yago5.n3</t>
+  </si>
+  <si>
+    <t>yago-yago1-spin.nt</t>
+  </si>
+  <si>
+    <t>yago-yago2-spin.nt</t>
+  </si>
+  <si>
+    <t>yago-yago3-spin.nt</t>
+  </si>
+  <si>
+    <t>yago-yago4-spin.nt</t>
+  </si>
+  <si>
+    <t>yago-yago5-spin.nt</t>
+  </si>
+  <si>
+    <t>yago-yago1-recsparql.txt</t>
+  </si>
+  <si>
+    <t>yago-yago2-recsparql.txt</t>
+  </si>
+  <si>
+    <t>yago-yago3-recsparql.txt</t>
+  </si>
+  <si>
+    <t>yago-yago4-recsparql.txt</t>
+  </si>
+  <si>
+    <t>yago-yago5-recsparql.txt</t>
+  </si>
+  <si>
+    <t>recsparql-load</t>
+  </si>
+  <si>
+    <t>load_distrib</t>
   </si>
 </sst>
 </file>
@@ -614,9 +797,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -674,7 +856,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'gmark_50-eye'!$A$41:$A$79</c:f>
+              <c:f>gmark!$A$41:$A$79</c:f>
               <c:strCache>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
@@ -799,7 +981,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'gmark_50-eye'!$F$41:$F$79</c:f>
+              <c:f>gmark!$F$41:$F$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -947,7 +1129,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'gmark_50-eye'!$O$41:$O$79</c:f>
+              <c:f>gmark!$O$41:$O$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
@@ -1095,7 +1277,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'gmark_50-eye'!$U$41:$U$70</c:f>
+              <c:f>gmark!$U$41:$U$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1266,7 +1448,7 @@
         <c:axId val="317026576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="500"/>
+          <c:max val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1342,7 +1524,759 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lmdb!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sin3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>lmdb!$F$41:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>51.598000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.548000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4BEF-4C42-B3EB-4A829385D3EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lmdb!$H$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>spin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>lmdb!$M$41:$M$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>35.820999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.723000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38.164999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4BEF-4C42-B3EB-4A829385D3EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lmdb!$O$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>recsparql</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>lmdb!$S$41:$S$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>61.304998041666664</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.962291499666669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.143806958666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4BEF-4C42-B3EB-4A829385D3EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="327607984"/>
+        <c:axId val="327621552"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="327607984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="327621552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="327621552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="327607984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yago!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sin3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>yago!$F$33:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>48.986999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.273000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.039000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.294000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58.574999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD56-AB4A-96EA-09F265966B05}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yago!$H$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>spin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>yago!$M$33:$M$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>52.012382290999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.022273290999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.510693334000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.015443165999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.754125291999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FD56-AB4A-96EA-09F265966B05}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>yago!$O$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>recsparql</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>yago!$S$33:$S$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60.094626333000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.166931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.852720667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.513591290999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.857941166999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FD56-AB4A-96EA-09F265966B05}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1896039888"/>
+        <c:axId val="327667600"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1896039888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="327667600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="327667600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1896039888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1442,7 +2376,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1986,6 +4006,88 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8BC3B10-47AA-5807-8931-2F0E7811051B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>255732</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>169142</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>325582</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>188191</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E8DFDF8-F19D-5A24-2D3D-EA703B5C456B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-nmo" connectionId="3" xr16:uid="{36FE3CBF-7CFB-144F-BD3C-F99FBC1279EB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -1996,6 +4098,30 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-eye" connectionId="1" xr16:uid="{B28165AC-629A-FD46-BA9E-572113DC25B6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb_recsparql_1" connectionId="5" xr16:uid="{2A698B41-D615-404D-8337-6C2818CFDAE3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb-spin" connectionId="6" xr16:uid="{4463E946-FA3D-6D40-AD0A-56D24E5E34B2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb-eye" connectionId="4" xr16:uid="{ADC41410-6788-9143-8CF5-2CAA91DF4846}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago-recsparql" connectionId="9" xr16:uid="{2ECA2510-95FC-0E49-A0C0-572203E357D6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago-spin" connectionId="10" xr16:uid="{663FA744-5A49-E04A-B4DA-4074CBDB55A9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago-eye" connectionId="8" xr16:uid="{EAF114E9-9722-4042-AF04-EFDCB19275B4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2318,7 +4444,7 @@
   <dimension ref="A6:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2340,143 +4466,26 @@
     <col min="19" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="21:21" x14ac:dyDescent="0.2">
       <c r="U6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="21:21" x14ac:dyDescent="0.2">
       <c r="U7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="U8" s="2"/>
+    <row r="8" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="U9" s="2"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+    <row r="9" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U9" s="1"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="1"/>
       <c r="H39" t="s">
         <v>125</v>
       </c>
@@ -2485,10 +4494,10 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>0</v>
       </c>
       <c r="C40" t="s">
@@ -2544,10 +4553,10 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>5</v>
       </c>
       <c r="C41">
@@ -2606,10 +4615,10 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42">
@@ -2668,10 +4677,10 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43">
@@ -2730,10 +4739,10 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44">
@@ -2792,10 +4801,10 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>13</v>
       </c>
       <c r="C45">
@@ -2854,10 +4863,10 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>15</v>
       </c>
       <c r="C46">
@@ -2916,10 +4925,10 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>17</v>
       </c>
       <c r="C47">
@@ -2978,10 +4987,10 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>18</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>19</v>
       </c>
       <c r="C48">
@@ -4839,15 +6848,663 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9D665C-2534-3847-B454-D62D9ED4F32D}">
-  <dimension ref="A1"/>
+  <dimension ref="A39:V43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>173</v>
+      </c>
+      <c r="H39" t="s">
+        <v>172</v>
+      </c>
+      <c r="O39" t="s">
+        <v>177</v>
+      </c>
+      <c r="V39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>160</v>
+      </c>
+      <c r="H40" t="s">
+        <v>82</v>
+      </c>
+      <c r="I40" t="s">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>178</v>
+      </c>
+      <c r="K40" t="s">
+        <v>127</v>
+      </c>
+      <c r="L40" t="s">
+        <v>128</v>
+      </c>
+      <c r="M40" t="s">
+        <v>160</v>
+      </c>
+      <c r="O40" t="s">
+        <v>82</v>
+      </c>
+      <c r="P40" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>128</v>
+      </c>
+      <c r="R40" t="s">
+        <v>200</v>
+      </c>
+      <c r="S40" t="s">
+        <v>160</v>
+      </c>
+      <c r="V40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="D41">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E41">
+        <v>50.962000000000003</v>
+      </c>
+      <c r="F41">
+        <f>SUM(C41:E41)</f>
+        <v>51.598000000000006</v>
+      </c>
+      <c r="H41" t="s">
+        <v>163</v>
+      </c>
+      <c r="I41" t="s">
+        <v>169</v>
+      </c>
+      <c r="J41">
+        <v>23</v>
+      </c>
+      <c r="K41">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="L41">
+        <v>12.72</v>
+      </c>
+      <c r="M41">
+        <f>SUM(J41:L41)</f>
+        <v>35.820999999999998</v>
+      </c>
+      <c r="O41" t="s">
+        <v>163</v>
+      </c>
+      <c r="P41" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q41">
+        <v>50.638331375</v>
+      </c>
+      <c r="R41">
+        <f>V41/3</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="S41">
+        <f>SUM(Q41:R41)</f>
+        <v>61.304998041666664</v>
+      </c>
+      <c r="V41">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="D42">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="E42">
+        <v>32.462000000000003</v>
+      </c>
+      <c r="F42">
+        <f t="shared" ref="F42:F43" si="0">SUM(C42:E42)</f>
+        <v>33.14</v>
+      </c>
+      <c r="H42" t="s">
+        <v>165</v>
+      </c>
+      <c r="I42" t="s">
+        <v>170</v>
+      </c>
+      <c r="J42">
+        <v>23</v>
+      </c>
+      <c r="K42">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L42">
+        <v>3.7189999999999999</v>
+      </c>
+      <c r="M42">
+        <f t="shared" ref="M42:M43" si="1">SUM(J42:L42)</f>
+        <v>26.723000000000003</v>
+      </c>
+      <c r="O42" t="s">
+        <v>165</v>
+      </c>
+      <c r="P42" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q42">
+        <v>17.295624833000002</v>
+      </c>
+      <c r="R42">
+        <f>V41/3</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="S42">
+        <f t="shared" ref="S42:S43" si="2">SUM(Q42:R42)</f>
+        <v>27.962291499666669</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>167</v>
+      </c>
+      <c r="B43" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="D43">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="E43">
+        <v>38.902000000000001</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>39.548000000000002</v>
+      </c>
+      <c r="H43" t="s">
+        <v>167</v>
+      </c>
+      <c r="I43" t="s">
+        <v>171</v>
+      </c>
+      <c r="J43">
+        <v>23</v>
+      </c>
+      <c r="K43">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L43">
+        <v>15.162000000000001</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="1"/>
+        <v>38.164999999999999</v>
+      </c>
+      <c r="O43" t="s">
+        <v>167</v>
+      </c>
+      <c r="P43" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q43">
+        <v>21.477140292000001</v>
+      </c>
+      <c r="R43">
+        <f>V41/3</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="2"/>
+        <v>32.143806958666666</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3B7BA1-0FD9-C84A-9CB0-1F3FBC24574F}">
+  <dimension ref="A31:U37"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>173</v>
+      </c>
+      <c r="H31" t="s">
+        <v>172</v>
+      </c>
+      <c r="O31" t="s">
+        <v>177</v>
+      </c>
+      <c r="U31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>160</v>
+      </c>
+      <c r="H32" t="s">
+        <v>82</v>
+      </c>
+      <c r="I32" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>178</v>
+      </c>
+      <c r="K32" t="s">
+        <v>127</v>
+      </c>
+      <c r="L32" t="s">
+        <v>128</v>
+      </c>
+      <c r="M32" t="s">
+        <v>160</v>
+      </c>
+      <c r="O32" t="s">
+        <v>82</v>
+      </c>
+      <c r="P32" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>128</v>
+      </c>
+      <c r="R32" t="s">
+        <v>200</v>
+      </c>
+      <c r="S32" t="s">
+        <v>160</v>
+      </c>
+      <c r="U32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" t="s">
+        <v>180</v>
+      </c>
+      <c r="C33">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="D33">
+        <v>7.8E-2</v>
+      </c>
+      <c r="E33">
+        <v>48.351999999999997</v>
+      </c>
+      <c r="F33">
+        <f>SUM(C33:E33)</f>
+        <v>48.986999999999995</v>
+      </c>
+      <c r="H33" t="s">
+        <v>179</v>
+      </c>
+      <c r="I33" t="s">
+        <v>189</v>
+      </c>
+      <c r="J33">
+        <v>42</v>
+      </c>
+      <c r="K33">
+        <v>0.103277416</v>
+      </c>
+      <c r="L33">
+        <v>9.9091048750000006</v>
+      </c>
+      <c r="M33">
+        <f>SUM(I33:L33)</f>
+        <v>52.012382290999994</v>
+      </c>
+      <c r="O33" t="s">
+        <v>179</v>
+      </c>
+      <c r="P33" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q33">
+        <v>49.494626332999999</v>
+      </c>
+      <c r="R33">
+        <f>U33/5</f>
+        <v>10.6</v>
+      </c>
+      <c r="S33">
+        <f>SUM(Q33:R33)</f>
+        <v>60.094626333000001</v>
+      </c>
+      <c r="U33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34">
+        <v>0.624</v>
+      </c>
+      <c r="D34">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E34">
+        <v>35.567</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F37" si="0">SUM(C34:E34)</f>
+        <v>36.273000000000003</v>
+      </c>
+      <c r="H34" t="s">
+        <v>181</v>
+      </c>
+      <c r="I34" t="s">
+        <v>190</v>
+      </c>
+      <c r="J34">
+        <v>41</v>
+      </c>
+      <c r="K34">
+        <v>4.3342500000000004E-3</v>
+      </c>
+      <c r="L34">
+        <v>1.7939040999999999E-2</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ref="M34:M37" si="1">SUM(I34:L34)</f>
+        <v>41.022273290999998</v>
+      </c>
+      <c r="O34" t="s">
+        <v>181</v>
+      </c>
+      <c r="P34" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q34">
+        <v>4.5669310000000003</v>
+      </c>
+      <c r="R34">
+        <f>U33/5</f>
+        <v>10.6</v>
+      </c>
+      <c r="S34">
+        <f t="shared" ref="S34:S37" si="2">SUM(Q34:R34)</f>
+        <v>15.166931</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35">
+        <v>0.622</v>
+      </c>
+      <c r="D35">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="E35">
+        <v>39.338000000000001</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>40.039000000000001</v>
+      </c>
+      <c r="H35" t="s">
+        <v>183</v>
+      </c>
+      <c r="I35" t="s">
+        <v>191</v>
+      </c>
+      <c r="J35">
+        <v>40</v>
+      </c>
+      <c r="K35">
+        <v>4.2229169999999996E-3</v>
+      </c>
+      <c r="L35">
+        <v>6.5064704170000001</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>46.510693334000003</v>
+      </c>
+      <c r="O35" t="s">
+        <v>183</v>
+      </c>
+      <c r="P35" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q35">
+        <v>20.252720666999998</v>
+      </c>
+      <c r="R35">
+        <f>U33/5</f>
+        <v>10.6</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="2"/>
+        <v>30.852720667</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>185</v>
+      </c>
+      <c r="B36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="D36">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E36">
+        <v>34.633000000000003</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>35.294000000000004</v>
+      </c>
+      <c r="H36" t="s">
+        <v>185</v>
+      </c>
+      <c r="I36" t="s">
+        <v>192</v>
+      </c>
+      <c r="J36">
+        <v>42</v>
+      </c>
+      <c r="K36">
+        <v>7.4632079999999998E-3</v>
+      </c>
+      <c r="L36">
+        <v>7.9799580000000005E-3</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>42.015443165999997</v>
+      </c>
+      <c r="O36" t="s">
+        <v>185</v>
+      </c>
+      <c r="P36" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q36">
+        <v>12.913591290999999</v>
+      </c>
+      <c r="R36">
+        <f>U33/5</f>
+        <v>10.6</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="2"/>
+        <v>23.513591290999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="D37">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E37">
+        <v>57.9</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>58.574999999999996</v>
+      </c>
+      <c r="H37" t="s">
+        <v>187</v>
+      </c>
+      <c r="I37" t="s">
+        <v>193</v>
+      </c>
+      <c r="J37">
+        <v>42</v>
+      </c>
+      <c r="K37">
+        <v>3.880667E-3</v>
+      </c>
+      <c r="L37">
+        <v>4.7502446249999997</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="1"/>
+        <v>46.754125291999998</v>
+      </c>
+      <c r="O37" t="s">
+        <v>187</v>
+      </c>
+      <c r="P37" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q37">
+        <v>73.257941166999998</v>
+      </c>
+      <c r="R37">
+        <f>U33/5</f>
+        <v>10.6</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="2"/>
+        <v>83.857941166999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add original, nmo queries for gmark
</commit_message>
<xml_diff>
--- a/SPIN-to-N3/test/run/cmp_times.xlsx
+++ b/SPIN-to-N3/test/run/cmp_times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DBD65A-A8DB-5843-BF52-BFF60E7004E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDE2FAB-8DC3-3E42-B233-57F72C7A204D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19840" xr2:uid="{94AE5E48-1175-4942-B1A9-4F55D3AD141D}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="gmark_50_eye" localSheetId="0">gmark!$A$40:$E$79</definedName>
     <definedName name="gmark_50_eye_forward" localSheetId="0">gmark!$H$40:$N$79</definedName>
-    <definedName name="gmark_50_nmo" localSheetId="0">gmark!$Q$40:$T$70</definedName>
+    <definedName name="gmark_50_nmo" localSheetId="0">gmark!$Q$40:$T$76</definedName>
     <definedName name="lmdb_eye" localSheetId="1">lmdb!$A$40:$E$43</definedName>
     <definedName name="lmdb_recsparql_1" localSheetId="1">lmdb!$O$40:$Q$43</definedName>
     <definedName name="lmdb_spin" localSheetId="1">lmdb!$H$40:$L$43</definedName>
@@ -85,7 +85,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{39F583D4-93FF-5146-994C-646A963F913B}" name="lmdb-eye" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-eye.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-eye.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -96,7 +96,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{FC45E0D5-6402-0341-AB3C-FB00067C91DF}" name="lmdb-recsparql" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-recsparql.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-recsparql.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -105,7 +105,7 @@
     </textPr>
   </connection>
   <connection id="6" xr16:uid="{1E6C00C3-C49D-0A41-B42A-D043CA0AB2F5}" name="lmdb-spin" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-spin.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-spin.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -119,7 +119,7 @@
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=gmark_50-eye;Extended Properties=&quot;&quot;" command="SELECT * FROM [gmark_50-eye]"/>
   </connection>
   <connection id="8" xr16:uid="{8E824083-4B73-C34C-B75C-E4C5FD24E1F4}" name="yago-eye" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-eye.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-eye.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -130,7 +130,7 @@
     </textPr>
   </connection>
   <connection id="9" xr16:uid="{A383D5A5-B79F-AB49-9812-02B5108CCB77}" name="yago-recsparql" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-recsparql.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-recsparql.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -139,7 +139,7 @@
     </textPr>
   </connection>
   <connection id="10" xr16:uid="{8BB0FA84-0301-4F41-98FC-E56B4A9EBBD1}" name="yago-spin" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-spin.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-spin.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="199">
   <si>
     <t>result_file</t>
   </si>
@@ -582,12 +582,6 @@
   </si>
   <si>
     <t>gmark_50-query-25.nmo</t>
-  </si>
-  <si>
-    <t>query-26</t>
-  </si>
-  <si>
-    <t>gmark_50-query-26.nmo</t>
   </si>
   <si>
     <t>gmark_50-query-28.nmo</t>
@@ -1277,10 +1271,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>gmark!$U$41:$U$70</c:f>
+              <c:f>gmark!$U$41:$U$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>1.6106374999999999</c:v>
                 </c:pt>
@@ -1302,73 +1296,70 @@
                 <c:pt idx="6">
                   <c:v>268.58956424999997</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.88204950000000004</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3.0853046260000001</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>1.6617014989999999</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.86864500099999997</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>1.386723624</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>0.89922341700000008</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>0.93875166700000001</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.74001541700000006</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>1.8858807070000001</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>3.255916042</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>0.98735270799999997</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>0.91344837499999998</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>0.99224574999999993</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>0.82145625100000008</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="25">
                   <c:v>0.84588579199999991</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="26">
                   <c:v>4.5417310840000003</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="28">
                   <c:v>0.95996925</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="29">
                   <c:v>8.2905520829999997</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="31">
                   <c:v>0.7789143340000001</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="32">
                   <c:v>0.82975004200000002</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="33">
                   <c:v>0.85052804199999998</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="34">
                   <c:v>2.8289343750000002</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="35">
                   <c:v>0.82691733199999995</c:v>
                 </c:pt>
               </c:numCache>
@@ -4443,8 +4434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB08BC1D-CD5B-B047-94E4-45C8752186BC}">
   <dimension ref="A6:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4468,12 +4459,12 @@
   <sheetData>
     <row r="6" spans="21:21" x14ac:dyDescent="0.2">
       <c r="U6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="21:21" x14ac:dyDescent="0.2">
       <c r="U7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="21:21" x14ac:dyDescent="0.2">
@@ -4510,7 +4501,7 @@
         <v>3</v>
       </c>
       <c r="F40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H40" t="s">
         <v>82</v>
@@ -4534,7 +4525,7 @@
         <v>3</v>
       </c>
       <c r="O40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q40" t="s">
         <v>82</v>
@@ -4549,7 +4540,7 @@
         <v>128</v>
       </c>
       <c r="U40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
@@ -5031,22 +5022,6 @@
         <f t="shared" si="1"/>
         <v>4.915</v>
       </c>
-      <c r="Q48" t="s">
-        <v>20</v>
-      </c>
-      <c r="R48" t="s">
-        <v>136</v>
-      </c>
-      <c r="S48">
-        <v>0.81154787500000003</v>
-      </c>
-      <c r="T48">
-        <v>7.0501624999999998E-2</v>
-      </c>
-      <c r="U48">
-        <f t="shared" si="2"/>
-        <v>0.88204950000000004</v>
-      </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -5094,20 +5069,20 @@
         <v>0.877</v>
       </c>
       <c r="Q49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="S49">
-        <v>0.86264254200000001</v>
+        <v>0.81154787500000003</v>
       </c>
       <c r="T49">
-        <v>2.222662084</v>
+        <v>7.0501624999999998E-2</v>
       </c>
       <c r="U49">
-        <f t="shared" si="2"/>
-        <v>3.0853046260000001</v>
+        <f>SUM(S49:T49)</f>
+        <v>0.88204950000000004</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
@@ -5156,20 +5131,20 @@
         <v>0.97899999999999998</v>
       </c>
       <c r="Q50" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="R50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S50">
-        <v>0.83709633299999997</v>
+        <v>0.86264254200000001</v>
       </c>
       <c r="T50">
-        <v>0.824605166</v>
+        <v>2.222662084</v>
       </c>
       <c r="U50">
-        <f t="shared" si="2"/>
-        <v>1.6617014989999999</v>
+        <f>SUM(S50:T50)</f>
+        <v>3.0853046260000001</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
@@ -5217,22 +5192,6 @@
         <f t="shared" si="1"/>
         <v>29.137999999999998</v>
       </c>
-      <c r="Q51" t="s">
-        <v>28</v>
-      </c>
-      <c r="R51" t="s">
-        <v>139</v>
-      </c>
-      <c r="S51">
-        <v>0.80226929199999997</v>
-      </c>
-      <c r="T51">
-        <v>6.6375709000000005E-2</v>
-      </c>
-      <c r="U51">
-        <f t="shared" si="2"/>
-        <v>0.86864500099999997</v>
-      </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -5280,20 +5239,20 @@
         <v>1.2210000000000001</v>
       </c>
       <c r="Q52" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="R52" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S52">
-        <v>0.877928916</v>
+        <v>0.83709633299999997</v>
       </c>
       <c r="T52">
-        <v>0.50879470800000004</v>
+        <v>0.824605166</v>
       </c>
       <c r="U52">
-        <f t="shared" si="2"/>
-        <v>1.386723624</v>
+        <f>SUM(S52:T52)</f>
+        <v>1.6617014989999999</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
@@ -5342,20 +5301,20 @@
         <v>0.90599999999999992</v>
       </c>
       <c r="Q53" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R53" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S53">
-        <v>0.81883462500000004</v>
+        <v>0.80226929199999997</v>
       </c>
       <c r="T53">
-        <v>8.0388792000000001E-2</v>
+        <v>6.6375709000000005E-2</v>
       </c>
       <c r="U53">
-        <f t="shared" si="2"/>
-        <v>0.89922341700000008</v>
+        <f>SUM(S53:T53)</f>
+        <v>0.86864500099999997</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
@@ -5404,20 +5363,20 @@
         <v>0.99599999999999989</v>
       </c>
       <c r="Q54" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="R54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S54">
-        <v>0.82156050000000003</v>
+        <v>0.877928916</v>
       </c>
       <c r="T54">
-        <v>0.117191167</v>
+        <v>0.50879470800000004</v>
       </c>
       <c r="U54">
-        <f t="shared" si="2"/>
-        <v>0.93875166700000001</v>
+        <f>SUM(S54:T54)</f>
+        <v>1.386723624</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
@@ -5466,20 +5425,20 @@
         <v>0.92599999999999982</v>
       </c>
       <c r="Q55" t="s">
-        <v>143</v>
+        <v>32</v>
       </c>
       <c r="R55" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="S55">
-        <v>0.72344200000000003</v>
+        <v>0.81883462500000004</v>
       </c>
       <c r="T55">
-        <v>1.6573417E-2</v>
+        <v>8.0388792000000001E-2</v>
       </c>
       <c r="U55">
-        <f t="shared" si="2"/>
-        <v>0.74001541700000006</v>
+        <f>SUM(S55:T55)</f>
+        <v>0.89922341700000008</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
@@ -5527,22 +5486,6 @@
         <f t="shared" si="1"/>
         <v>64.875</v>
       </c>
-      <c r="Q56" t="s">
-        <v>40</v>
-      </c>
-      <c r="R56" t="s">
-        <v>145</v>
-      </c>
-      <c r="S56">
-        <v>0.90139504100000001</v>
-      </c>
-      <c r="T56">
-        <v>0.98448566599999998</v>
-      </c>
-      <c r="U56">
-        <f t="shared" si="2"/>
-        <v>1.8858807070000001</v>
-      </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -5590,20 +5533,20 @@
         <v>0.95499999999999985</v>
       </c>
       <c r="Q57" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="R57" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="S57">
-        <v>0.82591416699999998</v>
+        <v>0.82156050000000003</v>
       </c>
       <c r="T57">
-        <v>2.4300018749999999</v>
+        <v>0.117191167</v>
       </c>
       <c r="U57">
-        <f t="shared" si="2"/>
-        <v>3.255916042</v>
+        <f>SUM(S57:T57)</f>
+        <v>0.93875166700000001</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
@@ -5651,22 +5594,6 @@
         <f t="shared" si="1"/>
         <v>90.146999999999991</v>
       </c>
-      <c r="Q58" t="s">
-        <v>44</v>
-      </c>
-      <c r="R58" t="s">
-        <v>147</v>
-      </c>
-      <c r="S58">
-        <v>0.83284329099999999</v>
-      </c>
-      <c r="T58">
-        <v>0.15450941700000001</v>
-      </c>
-      <c r="U58">
-        <f t="shared" si="2"/>
-        <v>0.98735270799999997</v>
-      </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -5714,20 +5641,20 @@
         <v>7.0760000000000005</v>
       </c>
       <c r="Q59" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="R59" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="S59">
-        <v>0.79981629200000004</v>
+        <v>0.90139504100000001</v>
       </c>
       <c r="T59">
-        <v>0.11363208299999999</v>
+        <v>0.98448566599999998</v>
       </c>
       <c r="U59">
-        <f t="shared" si="2"/>
-        <v>0.91344837499999998</v>
+        <f>SUM(S59:T59)</f>
+        <v>1.8858807070000001</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.2">
@@ -5776,20 +5703,20 @@
         <v>0.96199999999999986</v>
       </c>
       <c r="Q60" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R60" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="S60">
-        <v>0.80330212499999998</v>
+        <v>0.82591416699999998</v>
       </c>
       <c r="T60">
-        <v>0.188943625</v>
+        <v>2.4300018749999999</v>
       </c>
       <c r="U60">
-        <f t="shared" si="2"/>
-        <v>0.99224574999999993</v>
+        <f>SUM(S60:T60)</f>
+        <v>3.255916042</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
@@ -5838,20 +5765,20 @@
         <v>0.95299999999999985</v>
       </c>
       <c r="Q61" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R61" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="S61">
-        <v>0.77139304200000003</v>
+        <v>0.83284329099999999</v>
       </c>
       <c r="T61">
-        <v>5.0063208999999997E-2</v>
+        <v>0.15450941700000001</v>
       </c>
       <c r="U61">
-        <f t="shared" si="2"/>
-        <v>0.82145625100000008</v>
+        <f>SUM(S61:T61)</f>
+        <v>0.98735270799999997</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.2">
@@ -5900,20 +5827,20 @@
         <v>0.94799999999999995</v>
       </c>
       <c r="Q62" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="R62" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="S62">
-        <v>0.79697237499999996</v>
+        <v>0.79981629200000004</v>
       </c>
       <c r="T62">
-        <v>4.8913417000000001E-2</v>
+        <v>0.11363208299999999</v>
       </c>
       <c r="U62">
-        <f t="shared" si="2"/>
-        <v>0.84588579199999991</v>
+        <f>SUM(S62:T62)</f>
+        <v>0.91344837499999998</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
@@ -5962,20 +5889,20 @@
         <v>0.99699999999999989</v>
       </c>
       <c r="Q63" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="R63" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="S63">
-        <v>0.86832679199999996</v>
+        <v>0.80330212499999998</v>
       </c>
       <c r="T63">
-        <v>3.6734042919999998</v>
+        <v>0.188943625</v>
       </c>
       <c r="U63">
-        <f t="shared" si="2"/>
-        <v>4.5417310840000003</v>
+        <f>SUM(S63:T63)</f>
+        <v>0.99224574999999993</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
@@ -6024,20 +5951,20 @@
         <v>0.84899999999999998</v>
       </c>
       <c r="Q64" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="R64" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="S64">
-        <v>0.788181417</v>
+        <v>0.77139304200000003</v>
       </c>
       <c r="T64">
-        <v>0.171787833</v>
+        <v>5.0063208999999997E-2</v>
       </c>
       <c r="U64">
-        <f t="shared" si="2"/>
-        <v>0.95996925</v>
+        <f>SUM(S64:T64)</f>
+        <v>0.82145625100000008</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
@@ -6085,22 +6012,6 @@
         <f t="shared" si="1"/>
         <v>8.1579999999999995</v>
       </c>
-      <c r="Q65" t="s">
-        <v>62</v>
-      </c>
-      <c r="R65" t="s">
-        <v>154</v>
-      </c>
-      <c r="S65">
-        <v>0.83296495800000003</v>
-      </c>
-      <c r="T65">
-        <v>7.4575871249999999</v>
-      </c>
-      <c r="U65">
-        <f t="shared" si="2"/>
-        <v>8.2905520829999997</v>
-      </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -6148,20 +6059,20 @@
         <v>0.872</v>
       </c>
       <c r="Q66" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="R66" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="S66">
-        <v>0.74988362500000005</v>
+        <v>0.79697237499999996</v>
       </c>
       <c r="T66">
-        <v>2.9030708999999998E-2</v>
+        <v>4.8913417000000001E-2</v>
       </c>
       <c r="U66">
-        <f t="shared" si="2"/>
-        <v>0.7789143340000001</v>
+        <f>SUM(S66:T66)</f>
+        <v>0.84588579199999991</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
@@ -6210,20 +6121,20 @@
         <v>1.016</v>
       </c>
       <c r="Q67" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="R67" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="S67">
-        <v>0.76439299999999999</v>
+        <v>0.86832679199999996</v>
       </c>
       <c r="T67">
-        <v>6.5357042000000004E-2</v>
+        <v>3.6734042919999998</v>
       </c>
       <c r="U67">
-        <f t="shared" si="2"/>
-        <v>0.82975004200000002</v>
+        <f>SUM(S67:T67)</f>
+        <v>4.5417310840000003</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
@@ -6271,22 +6182,6 @@
         <f t="shared" si="1"/>
         <v>11.274000000000001</v>
       </c>
-      <c r="Q68" t="s">
-        <v>70</v>
-      </c>
-      <c r="R68" t="s">
-        <v>157</v>
-      </c>
-      <c r="S68">
-        <v>0.81260937499999997</v>
-      </c>
-      <c r="T68">
-        <v>3.7918667000000003E-2</v>
-      </c>
-      <c r="U68">
-        <f t="shared" si="2"/>
-        <v>0.85052804199999998</v>
-      </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -6334,20 +6229,20 @@
         <v>1.1439999999999999</v>
       </c>
       <c r="Q69" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="R69" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="S69">
-        <v>0.96779379200000004</v>
+        <v>0.788181417</v>
       </c>
       <c r="T69">
-        <v>1.8611405830000001</v>
+        <v>0.171787833</v>
       </c>
       <c r="U69">
-        <f t="shared" si="2"/>
-        <v>2.8289343750000002</v>
+        <f>SUM(S69:T69)</f>
+        <v>0.95996925</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
@@ -6396,20 +6291,20 @@
         <v>0.94</v>
       </c>
       <c r="Q70" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="R70" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="S70">
-        <v>0.78399529099999998</v>
+        <v>0.83296495800000003</v>
       </c>
       <c r="T70">
-        <v>4.2922041000000001E-2</v>
+        <v>7.4575871249999999</v>
       </c>
       <c r="U70">
-        <f t="shared" si="2"/>
-        <v>0.82691733199999995</v>
+        <f>SUM(S70:T70)</f>
+        <v>8.2905520829999997</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
@@ -6503,6 +6398,22 @@
         <f t="shared" si="1"/>
         <v>0.81899999999999995</v>
       </c>
+      <c r="Q72" t="s">
+        <v>66</v>
+      </c>
+      <c r="R72" t="s">
+        <v>153</v>
+      </c>
+      <c r="S72">
+        <v>0.74988362500000005</v>
+      </c>
+      <c r="T72">
+        <v>2.9030708999999998E-2</v>
+      </c>
+      <c r="U72">
+        <f>SUM(S72:T72)</f>
+        <v>0.7789143340000001</v>
+      </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -6549,6 +6460,22 @@
         <f t="shared" si="1"/>
         <v>0.82199999999999995</v>
       </c>
+      <c r="Q73" t="s">
+        <v>68</v>
+      </c>
+      <c r="R73" t="s">
+        <v>154</v>
+      </c>
+      <c r="S73">
+        <v>0.76439299999999999</v>
+      </c>
+      <c r="T73">
+        <v>6.5357042000000004E-2</v>
+      </c>
+      <c r="U73">
+        <f>SUM(S73:T73)</f>
+        <v>0.82975004200000002</v>
+      </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -6595,6 +6522,22 @@
         <f t="shared" si="1"/>
         <v>0.83899999999999997</v>
       </c>
+      <c r="Q74" t="s">
+        <v>70</v>
+      </c>
+      <c r="R74" t="s">
+        <v>155</v>
+      </c>
+      <c r="S74">
+        <v>0.81260937499999997</v>
+      </c>
+      <c r="T74">
+        <v>3.7918667000000003E-2</v>
+      </c>
+      <c r="U74">
+        <f>SUM(S74:T74)</f>
+        <v>0.85052804199999998</v>
+      </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -6641,6 +6584,22 @@
         <f t="shared" si="1"/>
         <v>1.2729999999999999</v>
       </c>
+      <c r="Q75" t="s">
+        <v>72</v>
+      </c>
+      <c r="R75" t="s">
+        <v>156</v>
+      </c>
+      <c r="S75">
+        <v>0.96779379200000004</v>
+      </c>
+      <c r="T75">
+        <v>1.8611405830000001</v>
+      </c>
+      <c r="U75">
+        <f>SUM(S75:T75)</f>
+        <v>2.8289343750000002</v>
+      </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -6686,6 +6645,22 @@
       <c r="O76">
         <f t="shared" si="1"/>
         <v>0.84699999999999986</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>74</v>
+      </c>
+      <c r="R76" t="s">
+        <v>157</v>
+      </c>
+      <c r="S76">
+        <v>0.78399529099999998</v>
+      </c>
+      <c r="T76">
+        <v>4.2922041000000001E-2</v>
+      </c>
+      <c r="U76">
+        <f>SUM(S76:T76)</f>
+        <v>0.82691733199999995</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -6836,8 +6811,8 @@
         <v>56.231128205128194</v>
       </c>
       <c r="U81">
-        <f>AVERAGE(U40:U70)</f>
-        <v>10.648783945833332</v>
+        <f>AVERAGE(U40:U76)</f>
+        <v>10.990465619241377</v>
       </c>
     </row>
   </sheetData>
@@ -6872,16 +6847,16 @@
   <sheetData>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O39" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="V39" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -6901,7 +6876,7 @@
         <v>3</v>
       </c>
       <c r="F40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H40" t="s">
         <v>82</v>
@@ -6910,7 +6885,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K40" t="s">
         <v>127</v>
@@ -6919,7 +6894,7 @@
         <v>128</v>
       </c>
       <c r="M40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O40" t="s">
         <v>82</v>
@@ -6931,21 +6906,21 @@
         <v>128</v>
       </c>
       <c r="R40" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="V40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C41">
         <v>0.56100000000000005</v>
@@ -6961,10 +6936,10 @@
         <v>51.598000000000006</v>
       </c>
       <c r="H41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J41">
         <v>23</v>
@@ -6980,10 +6955,10 @@
         <v>35.820999999999998</v>
       </c>
       <c r="O41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q41">
         <v>50.638331375</v>
@@ -7002,10 +6977,10 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C42">
         <v>0.59899999999999998</v>
@@ -7021,10 +6996,10 @@
         <v>33.14</v>
       </c>
       <c r="H42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I42" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J42">
         <v>23</v>
@@ -7040,10 +7015,10 @@
         <v>26.723000000000003</v>
       </c>
       <c r="O42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="P42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q42">
         <v>17.295624833000002</v>
@@ -7059,10 +7034,10 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C43">
         <v>0.56699999999999995</v>
@@ -7078,10 +7053,10 @@
         <v>39.548000000000002</v>
       </c>
       <c r="H43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I43" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J43">
         <v>23</v>
@@ -7097,10 +7072,10 @@
         <v>38.164999999999999</v>
       </c>
       <c r="O43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="P43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q43">
         <v>21.477140292000001</v>
@@ -7146,16 +7121,16 @@
   <sheetData>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="U31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
@@ -7175,7 +7150,7 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H32" t="s">
         <v>82</v>
@@ -7184,7 +7159,7 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K32" t="s">
         <v>127</v>
@@ -7193,7 +7168,7 @@
         <v>128</v>
       </c>
       <c r="M32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O32" t="s">
         <v>82</v>
@@ -7205,21 +7180,21 @@
         <v>128</v>
       </c>
       <c r="R32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="U32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C33">
         <v>0.55700000000000005</v>
@@ -7235,10 +7210,10 @@
         <v>48.986999999999995</v>
       </c>
       <c r="H33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J33">
         <v>42</v>
@@ -7254,10 +7229,10 @@
         <v>52.012382290999994</v>
       </c>
       <c r="O33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P33" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="Q33">
         <v>49.494626332999999</v>
@@ -7276,10 +7251,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C34">
         <v>0.624</v>
@@ -7295,10 +7270,10 @@
         <v>36.273000000000003</v>
       </c>
       <c r="H34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J34">
         <v>41</v>
@@ -7314,10 +7289,10 @@
         <v>41.022273290999998</v>
       </c>
       <c r="O34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="P34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="Q34">
         <v>4.5669310000000003</v>
@@ -7333,10 +7308,10 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B35" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C35">
         <v>0.622</v>
@@ -7352,10 +7327,10 @@
         <v>40.039000000000001</v>
       </c>
       <c r="H35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J35">
         <v>40</v>
@@ -7371,10 +7346,10 @@
         <v>46.510693334000003</v>
       </c>
       <c r="O35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Q35">
         <v>20.252720666999998</v>
@@ -7390,10 +7365,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C36">
         <v>0.58599999999999997</v>
@@ -7409,10 +7384,10 @@
         <v>35.294000000000004</v>
       </c>
       <c r="H36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I36" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J36">
         <v>42</v>
@@ -7428,10 +7403,10 @@
         <v>42.015443165999997</v>
       </c>
       <c r="O36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="P36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q36">
         <v>12.913591290999999</v>
@@ -7447,10 +7422,10 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C37">
         <v>0.58699999999999997</v>
@@ -7466,10 +7441,10 @@
         <v>58.574999999999996</v>
       </c>
       <c r="H37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I37" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J37">
         <v>42</v>
@@ -7485,10 +7460,10 @@
         <v>46.754125291999998</v>
       </c>
       <c r="O37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="P37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q37">
         <v>73.257941166999998</v>

</xml_diff>

<commit_message>
convert sparql to pp
</commit_message>
<xml_diff>
--- a/SPIN-to-N3/test/run/cmp_times.xlsx
+++ b/SPIN-to-N3/test/run/cmp_times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14F61B3-C24A-3441-A104-6E541B6F32C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA03B43-9688-A141-97FF-B320EC95A44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19840" activeTab="6" xr2:uid="{94AE5E48-1175-4942-B1A9-4F55D3AD141D}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="8" xr2:uid="{94AE5E48-1175-4942-B1A9-4F55D3AD141D}"/>
   </bookViews>
   <sheets>
     <sheet name="gmark-50" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="yago" sheetId="3" r:id="rId5"/>
     <sheet name="onto" sheetId="6" r:id="rId6"/>
     <sheet name="cmp" sheetId="7" r:id="rId7"/>
+    <sheet name="zika" sheetId="8" r:id="rId8"/>
+    <sheet name="dt" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="gmark_100_eye_forward_noDupl_resultList" localSheetId="1">'gmark-100'!$A$2:$G$42</definedName>
@@ -47,6 +49,15 @@
     <definedName name="yago_recsparql_1" localSheetId="4">yago!$T$41:$X$68</definedName>
     <definedName name="yago_spin" localSheetId="4">yago!$L$32:$P$37</definedName>
     <definedName name="yago_spin_1" localSheetId="4">yago!$L$41:$P$78</definedName>
+    <definedName name="zika_spin" localSheetId="7">zika!$E$5:$I$10</definedName>
+    <definedName name="zika_spin_1" localSheetId="7">zika!$E$17:$I$22</definedName>
+    <definedName name="zika_spin_2" localSheetId="7">zika!$P$5:$T$10</definedName>
+    <definedName name="zika_spin_3" localSheetId="7">zika!$P$17:$T$22</definedName>
+    <definedName name="zika_spin_5" localSheetId="7">zika!#REF!</definedName>
+    <definedName name="zika_spin_6" localSheetId="7">zika!$AA$17:$AI$21</definedName>
+    <definedName name="zika_spin_7" localSheetId="7">zika!$AA$29:$AI$34</definedName>
+    <definedName name="zika_spin_8" localSheetId="7">zika!$AA$5:$AE$10</definedName>
+    <definedName name="zika_spin_9" localSheetId="7">zika!$AA$30:$AE$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -211,7 +222,7 @@
     </textPr>
   </connection>
   <connection id="13" xr16:uid="{B9CFD8D9-A1A8-4F42-832B-C8C7C76D5CFA}" name="lmdb-eye1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-eye.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-eye.csv" comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -235,7 +246,7 @@
     </textPr>
   </connection>
   <connection id="15" xr16:uid="{7D6EE307-64A7-9342-85C1-950802A4CF91}" name="lmdb-recsparql1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-recsparql.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-recsparql.csv" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -255,7 +266,7 @@
     </textPr>
   </connection>
   <connection id="17" xr16:uid="{0602C752-BB48-7B4C-AE0E-073F02BC6D6E}" name="lmdb-spin1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-spin.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/lmdb-spin.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -305,7 +316,7 @@
     </textPr>
   </connection>
   <connection id="22" xr16:uid="{16C9C795-8279-FD4B-B76B-1B198530582C}" name="yago-eye1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-eye.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-eye.csv" comma="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -328,7 +339,7 @@
     </textPr>
   </connection>
   <connection id="24" xr16:uid="{AB77350C-9033-EA4E-A740-76635C71DF5A}" name="yago-recsparql1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-recsparql.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-recsparql.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -350,7 +361,103 @@
     </textPr>
   </connection>
   <connection id="26" xr16:uid="{1DB80AEC-8DC3-CE47-BF7A-676C73C201EC}" name="yago-spin1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-spin.csv" comma="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/yago-spin.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="27" xr16:uid="{117B4C59-22A1-304F-81ED-BE9AD7CFAAB6}" name="zika-spin" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/zika-spin.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="28" xr16:uid="{1ED72F78-A26E-BC4A-91EF-56410A441DA1}" name="zika-spin1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/zika-spin.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="29" xr16:uid="{F899F0B1-D851-8742-ACAA-86D99FA9A511}" name="zika-spin2" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/zika-spin.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="30" xr16:uid="{DFF503EC-3527-9047-B163-2583CDBA197B}" name="zika-spin3" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/zika-spin.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="31" xr16:uid="{C897FECC-5B61-8342-9B08-18B8C4F09348}" name="zika-spin4" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/zika-spin.csv" comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="32" xr16:uid="{89F5B1E0-A7A4-B749-9384-FA7CFB6CF6DB}" name="zika-spin6" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/zika-spin.csv" comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="33" xr16:uid="{E6D0DFA0-1D2F-D744-9CB2-25DC09D7AE2F}" name="zika-spin7" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/zika-spin.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="34" xr16:uid="{B15A6552-DAD1-7A4F-9D4F-832C5031EF8E}" name="zika-spin8" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/wvw/git/n3/sparql2n3/SPARQL-to-N3/SPIN-to-N3/test/run/times/zika-spin.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -364,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="647">
   <si>
     <t>result_file</t>
   </si>
@@ -2248,6 +2355,63 @@
   </si>
   <si>
     <t>(outlier)</t>
+  </si>
+  <si>
+    <t>(manual)</t>
+  </si>
+  <si>
+    <t>eye-fwd</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>exec</t>
+  </si>
+  <si>
+    <t>gen1000_pt1</t>
+  </si>
+  <si>
+    <t>gen1000_pt2</t>
+  </si>
+  <si>
+    <t>FULL</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>eye-bwd</t>
+  </si>
+  <si>
+    <t>SUBCLASS</t>
+  </si>
+  <si>
+    <t>zika-queries-all-optim1</t>
+  </si>
+  <si>
+    <t>zika</t>
+  </si>
+  <si>
+    <t>SPIN</t>
+  </si>
+  <si>
+    <t>zika-queries-all-red-optim</t>
+  </si>
+  <si>
+    <t>zika-queries-all-red-optim-sympt</t>
+  </si>
+  <si>
+    <t>gen1000_pt2 (2 extra conditions)</t>
+  </si>
+  <si>
+    <t>gen1000_pt2 (4 extra conditions)</t>
+  </si>
+  <si>
+    <t>gen1000_pt2 (6 extra conditions)</t>
+  </si>
+  <si>
+    <t>gen1000_pt2 (10 extra conditions)</t>
   </si>
 </sst>
 </file>
@@ -2307,12 +2471,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4910,6 +5074,325 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>sin3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(zika!$Z$13,zika!$Z$20,zika!$Z$34,zika!$Z$44,zika!$Z$50)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF0D-934D-9BEA-DE72C2A33424}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>spinrdf</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(zika!$AE$12,zika!$AE$25,zika!$AE$37,zika!$AE$43,zika!$AE$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.9267903834000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3693438834000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6989804496000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6912108339999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.906339209</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF0D-934D-9BEA-DE72C2A33424}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="712068048"/>
+        <c:axId val="712069760"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="712068048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712069760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="712069760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="712068048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5071,6 +5554,46 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7625,6 +8148,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7820,12 +8859,53 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>923192</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>376115</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>77176</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98ECCD3-6E95-5E9A-3137-DCBB6C73DBD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-nmo-forward-noDupl-resultPred" connectionId="10" xr16:uid="{75D6F480-C9B6-F54F-BC7D-4EDFA8EF684A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-eye-forward" connectionId="6" xr16:uid="{DD555A69-605C-4846-A691-4BE700C2572F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_100-nmo" connectionId="3" xr16:uid="{CECCB2E0-31F9-C44B-AB87-2D7BCC37CDA1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_100-eye-forward-noDupl-resultList" connectionId="1" xr16:uid="{E1D5B883-CD8D-9748-A882-6344BD91672C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7833,55 +8913,55 @@
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb-eye" connectionId="12" xr16:uid="{ADC41410-6788-9143-8CF5-2CAA91DF4846}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb_recsparql_1" connectionId="14" xr16:uid="{2A698B41-D615-404D-8337-6C2818CFDAE3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb_eye_1" connectionId="13" xr16:uid="{3D6F8494-08AC-8B4F-BFE2-413FA3F48786}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb-spin" connectionId="16" xr16:uid="{4463E946-FA3D-6D40-AD0A-56D24E5E34B2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb-recsparql" connectionId="15" xr16:uid="{360EB3FC-F1AA-DD46-B053-BE0CA8973F6C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb_spin_1" connectionId="17" xr16:uid="{4F218573-9E55-1C45-902D-4BEC71408E69}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb-eye" connectionId="12" xr16:uid="{ADC41410-6788-9143-8CF5-2CAA91DF4846}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago_recsparql_1" connectionId="24" xr16:uid="{31900917-82D5-A44C-A7A9-CAA85B8F5555}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb_recsparql_1" connectionId="14" xr16:uid="{2A698B41-D615-404D-8337-6C2818CFDAE3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="lmdb-spin" connectionId="16" xr16:uid="{4463E946-FA3D-6D40-AD0A-56D24E5E34B2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago_eye_1" connectionId="22" xr16:uid="{DD08B35E-7E1F-1949-B2D3-AAADC27A7581}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago_recsparql_1" connectionId="24" xr16:uid="{31900917-82D5-A44C-A7A9-CAA85B8F5555}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-eye-forward-noDupl" connectionId="7" xr16:uid="{E198AD8C-E518-384B-AE3D-AAE2BCC7D909}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-nmo" connectionId="9" xr16:uid="{36FE3CBF-7CFB-144F-BD3C-F99FBC1279EB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago-spin" connectionId="25" xr16:uid="{663FA744-5A49-E04A-B4DA-4074CBDB55A9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago_spin_1" connectionId="26" xr16:uid="{618EA0EE-4303-9844-96CA-0C592A1ABE89}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago-eye" connectionId="21" xr16:uid="{EAF114E9-9722-4042-AF04-EFDCB19275B4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago-recsparql" connectionId="23" xr16:uid="{2ECA2510-95FC-0E49-A0C0-572203E357D6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="yago-spin" connectionId="25" xr16:uid="{663FA744-5A49-E04A-B4DA-4074CBDB55A9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7892,32 +8972,64 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="owl2rl_eye" connectionId="18" xr16:uid="{5ED76186-EAAC-BB43-A972-C13CD126248C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="zika_spin_6" connectionId="31" xr16:uid="{6B2CDAD2-69BF-8145-AF96-540C61BF6E70}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="zika_spin_3" connectionId="30" xr16:uid="{BA603AA5-E821-5B40-9932-0C4110E1B49B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="zika_spin_2" connectionId="29" xr16:uid="{E2706558-5778-8649-AA8D-19470951E055}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="zika_spin_9" connectionId="34" xr16:uid="{2680075E-0FE6-914E-BCF1-9B8EA1DA1B6D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-eye" connectionId="5" xr16:uid="{B28165AC-629A-FD46-BA9E-572113DC25B6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="zika_spin_8" connectionId="33" xr16:uid="{38A9C34C-6FFA-464A-A156-AEAB70F12BF8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="zika_spin_1" connectionId="28" xr16:uid="{F3D63AB9-DF1F-0141-8C76-4148A0216DF5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="zika_spin_7" connectionId="32" xr16:uid="{35E00072-0B94-544B-98C2-8A99BCBE1A7E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="zika-spin" connectionId="27" xr16:uid="{9B602903-8CEB-AB43-A2D6-BF7A7200EDE7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-eye-forward-noDupl" connectionId="7" xr16:uid="{E198AD8C-E518-384B-AE3D-AAE2BCC7D909}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-eye-forward-noDupl-resultList" connectionId="8" xr16:uid="{9288756C-4130-404A-ABA8-4A7C61B439A7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-eye-forward" connectionId="6" xr16:uid="{DD555A69-605C-4846-A691-4BE700C2572F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-nmo" connectionId="9" xr16:uid="{36FE3CBF-7CFB-144F-BD3C-F99FBC1279EB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_50-nmo-forward-noDupl-resultPred" connectionId="10" xr16:uid="{75D6F480-C9B6-F54F-BC7D-4EDFA8EF684A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_100-eye-forward-noDupl-resultList" connectionId="1" xr16:uid="{E1D5B883-CD8D-9748-A882-6344BD91672C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_100-nmo-cnst" connectionId="4" xr16:uid="{2B4A541C-6204-1440-925A-1AE9E0EF838F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_100-nmo-cnst" connectionId="4" xr16:uid="{2B4A541C-6204-1440-925A-1AE9E0EF838F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_100-eye-forward-noDupl-resultList-cnst" connectionId="2" xr16:uid="{1A1E911C-3D2C-7F46-8FD1-4B2DFD3A6018}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_100-eye-forward-noDupl-resultList-cnst" connectionId="2" xr16:uid="{1A1E911C-3D2C-7F46-8FD1-4B2DFD3A6018}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="gmark_100-nmo" connectionId="3" xr16:uid="{CECCB2E0-31F9-C44B-AB87-2D7BCC37CDA1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17643,7 +18755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9D665C-2534-3847-B454-D62D9ED4F32D}">
   <dimension ref="A39:Z70"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
@@ -18889,7 +20001,7 @@
         <v>0.58399999999999996</v>
       </c>
       <c r="D65">
-        <f t="shared" ref="D65:H65" si="7">AVERAGE(D60:D64)</f>
+        <f t="shared" ref="D65:G65" si="7">AVERAGE(D60:D64)</f>
         <v>8.2400000000000001E-2</v>
       </c>
       <c r="E65">
@@ -19009,8 +20121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3B7BA1-0FD9-C84A-9CB0-1F3FBC24574F}">
   <dimension ref="A31:Y79"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView topLeftCell="A52" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20955,6 +22067,12 @@
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>628</v>
+      </c>
+      <c r="G73">
+        <v>12221</v>
+      </c>
       <c r="O73">
         <f>AVERAGE(O68:O72)</f>
         <v>2.9799831999999999E-3</v>
@@ -20974,6 +22092,9 @@
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>12361</v>
+      </c>
       <c r="L74" t="s">
         <v>183</v>
       </c>
@@ -20995,6 +22116,9 @@
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>12347</v>
+      </c>
       <c r="L75" t="s">
         <v>183</v>
       </c>
@@ -21012,6 +22136,9 @@
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>12304</v>
+      </c>
       <c r="L76" t="s">
         <v>183</v>
       </c>
@@ -21029,6 +22156,13 @@
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>12382</v>
+      </c>
+      <c r="H77">
+        <f>AVERAGE(G73:G77)</f>
+        <v>12323</v>
+      </c>
       <c r="L77" t="s">
         <v>183</v>
       </c>
@@ -25460,13 +26594,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33B9EE1-F568-0443-9C67-EE695BB8A0E7}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -25475,135 +26610,147 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>607</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>611</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" t="s">
         <v>606</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>608</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" t="s">
         <v>609</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" t="s">
         <v>611</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" t="s">
         <v>606</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" t="s">
         <v>609</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>610</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>599</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>31</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <v>0.1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4">
         <v>20.100000000000001</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>26.9</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4">
         <v>0.06</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4">
         <v>12</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>75.400000000000006</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4">
         <v>65.7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>600</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5">
+      <c r="B5" s="5"/>
+      <c r="C5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <v>0.08</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
         <v>2.4</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5">
+      <c r="F5" s="5"/>
+      <c r="G5">
         <v>0.02</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5">
         <v>3.9</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5">
+      <c r="I5" s="5"/>
+      <c r="J5">
         <v>18.399999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>601</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5">
+      <c r="B6" s="5"/>
+      <c r="C6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <v>0.08</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
         <v>9</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5">
+      <c r="F6" s="5"/>
+      <c r="G6">
         <v>0.02</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6">
         <v>19.5</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5">
+      <c r="I6" s="5"/>
+      <c r="J6">
         <v>24.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f>AVERAGE(E4:E6)</f>
+        <v>10.5</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(H4:H6)</f>
+        <v>11.799999999999999</v>
+      </c>
+      <c r="J7">
+        <f>AVERAGE(J4:J6)</f>
+        <v>36.199999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -25612,195 +26759,207 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
         <v>607</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>611</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" t="s">
         <v>606</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>608</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" t="s">
         <v>609</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" t="s">
         <v>611</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" t="s">
         <v>606</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" t="s">
         <v>609</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" t="s">
         <v>610</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>599</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>36.1</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12">
         <v>0.08</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12">
         <v>14.3</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>44.9</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12">
         <v>0.02</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12">
         <v>7.5</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>113686</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12">
         <v>50.2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>600</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5">
+      <c r="B13" s="5"/>
+      <c r="C13">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13">
         <v>0.08</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13">
         <v>1.5</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="5">
+      <c r="F13" s="5"/>
+      <c r="G13">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13">
         <v>0.01</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5">
+      <c r="I13" s="5"/>
+      <c r="J13">
         <v>3.2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>601</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5">
+      <c r="B14" s="5"/>
+      <c r="C14">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14">
         <v>0.08</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14">
         <v>5</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="5">
+      <c r="F14" s="5"/>
+      <c r="G14">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14">
         <v>2.8</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5">
+      <c r="I14" s="5"/>
+      <c r="J14">
         <v>22.4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>602</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5">
+      <c r="B15" s="5"/>
+      <c r="C15">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15">
         <v>0.4</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="5">
+      <c r="F15" s="5"/>
+      <c r="G15">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5">
+      <c r="I15" s="5"/>
+      <c r="J15">
         <v>14.4</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>603</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5">
+      <c r="B16" s="5"/>
+      <c r="C16">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16">
         <v>0.08</v>
       </c>
-      <c r="E16" s="5">
-        <v>23.5</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="5">
+      <c r="E16">
+        <v>12.3</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5">
+      <c r="I16" s="5"/>
+      <c r="J16">
         <v>83.2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f>AVERAGE(E12:E16)</f>
+        <v>6.7</v>
+      </c>
+      <c r="H17">
+        <f>AVERAGE(H12:H16)</f>
+        <v>3.0827999999999998</v>
+      </c>
+      <c r="J17">
+        <f>AVERAGE(J12:J16)</f>
+        <v>34.680000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>621</v>
       </c>
@@ -25811,83 +26970,78 @@
         <v>607</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>616</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>9.4</v>
       </c>
-      <c r="C21">
-        <v>13.5</v>
-      </c>
-      <c r="D21">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="4">
+        <v>13.2</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>615</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>229</v>
       </c>
-      <c r="C22">
-        <v>32</v>
-      </c>
-      <c r="D22">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="4">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>617</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>0.01</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>0.6</v>
       </c>
-      <c r="D23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>618</v>
       </c>
-      <c r="B24">
-        <v>0.5</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C24" s="4">
         <v>1.8</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>619</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4">
         <v>0.8</v>
       </c>
-      <c r="C25">
-        <v>3.7</v>
-      </c>
-      <c r="D25">
-        <v>6.4</v>
+      <c r="C25" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="D25" s="4">
+        <v>5.9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F12:F16"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:J2"/>
@@ -25895,7 +27049,1565 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F12:F16"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED038D2-68C7-424A-A7EB-CD00A4AEC8F0}">
+  <dimension ref="A1:AE50"/>
+  <sheetViews>
+    <sheetView topLeftCell="AE4" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
+      <selection activeCell="Z51" sqref="Z51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>634</v>
+      </c>
+      <c r="L1" t="s">
+        <v>635</v>
+      </c>
+      <c r="W1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>632</v>
+      </c>
+      <c r="L3" t="s">
+        <v>632</v>
+      </c>
+      <c r="W3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>629</v>
+      </c>
+      <c r="C4" t="s">
+        <v>636</v>
+      </c>
+      <c r="E4" t="s">
+        <v>640</v>
+      </c>
+      <c r="L4" t="s">
+        <v>629</v>
+      </c>
+      <c r="N4" t="s">
+        <v>636</v>
+      </c>
+      <c r="P4" t="s">
+        <v>640</v>
+      </c>
+      <c r="W4" t="s">
+        <v>629</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>630</v>
+      </c>
+      <c r="B5" t="s">
+        <v>631</v>
+      </c>
+      <c r="C5" t="s">
+        <v>630</v>
+      </c>
+      <c r="D5" t="s">
+        <v>631</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" t="s">
+        <v>126</v>
+      </c>
+      <c r="L5" t="s">
+        <v>630</v>
+      </c>
+      <c r="M5" t="s">
+        <v>631</v>
+      </c>
+      <c r="N5" t="s">
+        <v>630</v>
+      </c>
+      <c r="O5" t="s">
+        <v>631</v>
+      </c>
+      <c r="P5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>174</v>
+      </c>
+      <c r="S5" t="s">
+        <v>125</v>
+      </c>
+      <c r="T5" t="s">
+        <v>126</v>
+      </c>
+      <c r="W5" t="s">
+        <v>630</v>
+      </c>
+      <c r="X5" t="s">
+        <v>631</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>631</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>13191</v>
+      </c>
+      <c r="C6">
+        <v>97</v>
+      </c>
+      <c r="D6">
+        <v>9438</v>
+      </c>
+      <c r="E6" t="s">
+        <v>638</v>
+      </c>
+      <c r="F6" t="s">
+        <v>639</v>
+      </c>
+      <c r="G6">
+        <v>0.35160420799999997</v>
+      </c>
+      <c r="H6">
+        <v>0.153550042</v>
+      </c>
+      <c r="I6">
+        <v>0.73194400000000004</v>
+      </c>
+      <c r="L6">
+        <v>56</v>
+      </c>
+      <c r="M6">
+        <v>586</v>
+      </c>
+      <c r="N6">
+        <v>58</v>
+      </c>
+      <c r="O6">
+        <v>10</v>
+      </c>
+      <c r="P6" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>639</v>
+      </c>
+      <c r="R6">
+        <v>0.31914433399999997</v>
+      </c>
+      <c r="S6">
+        <v>0.15587662499999999</v>
+      </c>
+      <c r="T6">
+        <v>0.46617245800000001</v>
+      </c>
+      <c r="W6">
+        <v>1292</v>
+      </c>
+      <c r="X6">
+        <v>3809</v>
+      </c>
+      <c r="Y6">
+        <v>1378</v>
+      </c>
+      <c r="Z6">
+        <v>833</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC6">
+        <v>1.875621875</v>
+      </c>
+      <c r="AD6">
+        <v>0.124335167</v>
+      </c>
+      <c r="AE6">
+        <v>6.2882302499999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>13118</v>
+      </c>
+      <c r="C7">
+        <v>95</v>
+      </c>
+      <c r="D7">
+        <v>9482</v>
+      </c>
+      <c r="E7" t="s">
+        <v>638</v>
+      </c>
+      <c r="F7" t="s">
+        <v>639</v>
+      </c>
+      <c r="G7">
+        <v>2.8558541999999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>1.9522333999999999E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.40162170800000002</v>
+      </c>
+      <c r="L7">
+        <v>56</v>
+      </c>
+      <c r="M7">
+        <v>604</v>
+      </c>
+      <c r="N7">
+        <v>57</v>
+      </c>
+      <c r="O7">
+        <v>9</v>
+      </c>
+      <c r="P7" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>639</v>
+      </c>
+      <c r="R7">
+        <v>1.8213958999999998E-2</v>
+      </c>
+      <c r="S7">
+        <v>1.5333375E-2</v>
+      </c>
+      <c r="T7">
+        <v>0.26147358399999998</v>
+      </c>
+      <c r="W7">
+        <v>1292</v>
+      </c>
+      <c r="X7">
+        <v>3762</v>
+      </c>
+      <c r="Y7">
+        <v>1374</v>
+      </c>
+      <c r="Z7">
+        <v>816</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC7">
+        <v>1.3666083330000001</v>
+      </c>
+      <c r="AD7">
+        <v>2.0661790999999999E-2</v>
+      </c>
+      <c r="AE7">
+        <v>5.8965268340000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>13104</v>
+      </c>
+      <c r="C8">
+        <v>97</v>
+      </c>
+      <c r="D8">
+        <v>9252</v>
+      </c>
+      <c r="E8" t="s">
+        <v>638</v>
+      </c>
+      <c r="F8" t="s">
+        <v>639</v>
+      </c>
+      <c r="G8">
+        <v>2.4120209E-2</v>
+      </c>
+      <c r="H8">
+        <v>1.6484875E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.43024475000000001</v>
+      </c>
+      <c r="L8">
+        <v>54</v>
+      </c>
+      <c r="M8">
+        <v>592</v>
+      </c>
+      <c r="N8">
+        <v>57</v>
+      </c>
+      <c r="O8">
+        <v>9</v>
+      </c>
+      <c r="P8" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>639</v>
+      </c>
+      <c r="R8">
+        <v>1.097425E-2</v>
+      </c>
+      <c r="S8">
+        <v>1.181975E-2</v>
+      </c>
+      <c r="T8">
+        <v>0.244943416</v>
+      </c>
+      <c r="W8">
+        <v>1325</v>
+      </c>
+      <c r="X8">
+        <v>3743</v>
+      </c>
+      <c r="Y8">
+        <v>1346</v>
+      </c>
+      <c r="Z8">
+        <v>853</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC8">
+        <v>1.364495459</v>
+      </c>
+      <c r="AD8">
+        <v>1.3234958E-2</v>
+      </c>
+      <c r="AE8">
+        <v>5.888289125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>93</v>
+      </c>
+      <c r="B9">
+        <v>13158</v>
+      </c>
+      <c r="C9">
+        <v>97</v>
+      </c>
+      <c r="D9">
+        <v>9428</v>
+      </c>
+      <c r="E9" t="s">
+        <v>638</v>
+      </c>
+      <c r="F9" t="s">
+        <v>639</v>
+      </c>
+      <c r="G9">
+        <v>2.2252417E-2</v>
+      </c>
+      <c r="H9">
+        <v>1.1365333E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.50993891700000005</v>
+      </c>
+      <c r="L9">
+        <v>54</v>
+      </c>
+      <c r="M9">
+        <v>606</v>
+      </c>
+      <c r="N9">
+        <v>58</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+      <c r="P9" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>639</v>
+      </c>
+      <c r="R9">
+        <v>1.1752667E-2</v>
+      </c>
+      <c r="S9">
+        <v>1.0353083000000001E-2</v>
+      </c>
+      <c r="T9">
+        <v>0.21843095800000001</v>
+      </c>
+      <c r="W9">
+        <v>1339</v>
+      </c>
+      <c r="X9">
+        <v>3734</v>
+      </c>
+      <c r="Y9">
+        <v>1364</v>
+      </c>
+      <c r="Z9">
+        <v>835</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC9">
+        <v>1.440812875</v>
+      </c>
+      <c r="AD9">
+        <v>1.2454042E-2</v>
+      </c>
+      <c r="AE9">
+        <v>5.8960779170000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>13299</v>
+      </c>
+      <c r="C10">
+        <v>93</v>
+      </c>
+      <c r="D10">
+        <v>9431</v>
+      </c>
+      <c r="E10" t="s">
+        <v>638</v>
+      </c>
+      <c r="F10" t="s">
+        <v>639</v>
+      </c>
+      <c r="G10">
+        <v>2.7418667000000001E-2</v>
+      </c>
+      <c r="H10">
+        <v>1.0735082999999999E-2</v>
+      </c>
+      <c r="I10">
+        <v>0.38979837499999997</v>
+      </c>
+      <c r="L10">
+        <v>54</v>
+      </c>
+      <c r="M10">
+        <v>600</v>
+      </c>
+      <c r="N10">
+        <v>59</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>639</v>
+      </c>
+      <c r="R10">
+        <v>9.7890000000000008E-3</v>
+      </c>
+      <c r="S10">
+        <v>1.0381166000000001E-2</v>
+      </c>
+      <c r="T10">
+        <v>0.13730800000000001</v>
+      </c>
+      <c r="W10">
+        <v>1330</v>
+      </c>
+      <c r="X10">
+        <v>3738</v>
+      </c>
+      <c r="Y10">
+        <v>1391</v>
+      </c>
+      <c r="Z10">
+        <v>840</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC10">
+        <v>1.361814166</v>
+      </c>
+      <c r="AD10">
+        <v>1.0321333E-2</v>
+      </c>
+      <c r="AE10">
+        <v>5.6648277909999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f>AVERAGE(A9:A10)</f>
+        <v>91.5</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B6:B10)</f>
+        <v>13174</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C6:C10)</f>
+        <v>95.8</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D6:D10)</f>
+        <v>9406.2000000000007</v>
+      </c>
+      <c r="G12">
+        <f>AVERAGE(G6:G10)</f>
+        <v>9.0790808600000009E-2</v>
+      </c>
+      <c r="H12">
+        <f>AVERAGE(H6:H10)</f>
+        <v>4.2331533400000003E-2</v>
+      </c>
+      <c r="I12">
+        <f>AVERAGE(I6:I10)</f>
+        <v>0.49270955</v>
+      </c>
+      <c r="L12">
+        <f>AVERAGE(L6:L10)</f>
+        <v>54.8</v>
+      </c>
+      <c r="M12">
+        <f>AVERAGE(M6:M10)</f>
+        <v>597.6</v>
+      </c>
+      <c r="N12">
+        <f>AVERAGE(N6:N10)</f>
+        <v>57.8</v>
+      </c>
+      <c r="O12">
+        <f>AVERAGE(O6:O10)</f>
+        <v>9.6</v>
+      </c>
+      <c r="R12">
+        <f>AVERAGE(R6:R10)</f>
+        <v>7.3974841999999999E-2</v>
+      </c>
+      <c r="S12">
+        <f>AVERAGE(S6:S10)</f>
+        <v>4.0752799800000003E-2</v>
+      </c>
+      <c r="T12">
+        <f>AVERAGE(T6:T10)</f>
+        <v>0.2656656832</v>
+      </c>
+      <c r="W12">
+        <f>AVERAGE(W6:W10)</f>
+        <v>1315.6</v>
+      </c>
+      <c r="X12">
+        <f>AVERAGE(X6:X10)</f>
+        <v>3757.2</v>
+      </c>
+      <c r="Y12">
+        <f>AVERAGE(Y6:Y10)</f>
+        <v>1370.6</v>
+      </c>
+      <c r="Z12">
+        <f>AVERAGE(Z6:Z10)</f>
+        <v>835.4</v>
+      </c>
+      <c r="AC12">
+        <f>AVERAGE(AC6:AC10)</f>
+        <v>1.4818705416</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" ref="AD12:AE12" si="0">AVERAGE(AD6:AD10)</f>
+        <v>3.6201458199999995E-2</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="0"/>
+        <v>5.9267903834000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="Z13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>633</v>
+      </c>
+      <c r="L15" t="s">
+        <v>633</v>
+      </c>
+      <c r="W15" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>629</v>
+      </c>
+      <c r="C16" t="s">
+        <v>636</v>
+      </c>
+      <c r="E16" t="s">
+        <v>640</v>
+      </c>
+      <c r="L16" t="s">
+        <v>629</v>
+      </c>
+      <c r="N16" t="s">
+        <v>636</v>
+      </c>
+      <c r="P16" t="s">
+        <v>640</v>
+      </c>
+      <c r="W16" t="s">
+        <v>629</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>630</v>
+      </c>
+      <c r="B17" t="s">
+        <v>631</v>
+      </c>
+      <c r="C17" t="s">
+        <v>630</v>
+      </c>
+      <c r="D17" t="s">
+        <v>631</v>
+      </c>
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" t="s">
+        <v>126</v>
+      </c>
+      <c r="L17" t="s">
+        <v>630</v>
+      </c>
+      <c r="M17" t="s">
+        <v>631</v>
+      </c>
+      <c r="N17" t="s">
+        <v>630</v>
+      </c>
+      <c r="O17" t="s">
+        <v>631</v>
+      </c>
+      <c r="P17" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>174</v>
+      </c>
+      <c r="S17" t="s">
+        <v>125</v>
+      </c>
+      <c r="T17" t="s">
+        <v>126</v>
+      </c>
+      <c r="W17" t="s">
+        <v>630</v>
+      </c>
+      <c r="X17" t="s">
+        <v>631</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>631</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>148</v>
+      </c>
+      <c r="B18">
+        <v>32241</v>
+      </c>
+      <c r="C18">
+        <v>153</v>
+      </c>
+      <c r="D18">
+        <v>228109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>638</v>
+      </c>
+      <c r="F18" t="s">
+        <v>639</v>
+      </c>
+      <c r="G18">
+        <v>0.38461433299999997</v>
+      </c>
+      <c r="H18">
+        <v>0.14694125</v>
+      </c>
+      <c r="I18">
+        <v>1.1187339160000001</v>
+      </c>
+      <c r="L18">
+        <v>81</v>
+      </c>
+      <c r="M18">
+        <v>1770</v>
+      </c>
+      <c r="N18">
+        <v>85</v>
+      </c>
+      <c r="O18">
+        <v>427</v>
+      </c>
+      <c r="P18" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>639</v>
+      </c>
+      <c r="R18">
+        <v>0.34408833300000002</v>
+      </c>
+      <c r="S18">
+        <v>0.144904375</v>
+      </c>
+      <c r="T18">
+        <v>0.99759366699999996</v>
+      </c>
+      <c r="Y18">
+        <v>1530</v>
+      </c>
+      <c r="Z18">
+        <v>1112</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC18">
+        <v>1.7598128749999999</v>
+      </c>
+      <c r="AD18">
+        <v>0.13678758399999999</v>
+      </c>
+      <c r="AE18">
+        <v>5.5002314999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>150</v>
+      </c>
+      <c r="B19">
+        <v>31985</v>
+      </c>
+      <c r="E19" t="s">
+        <v>638</v>
+      </c>
+      <c r="F19" t="s">
+        <v>639</v>
+      </c>
+      <c r="G19">
+        <v>5.4258458000000002E-2</v>
+      </c>
+      <c r="H19">
+        <v>1.8794542000000001E-2</v>
+      </c>
+      <c r="I19">
+        <v>1.341445958</v>
+      </c>
+      <c r="L19">
+        <v>82</v>
+      </c>
+      <c r="M19">
+        <v>1717</v>
+      </c>
+      <c r="N19">
+        <v>87</v>
+      </c>
+      <c r="O19">
+        <v>441</v>
+      </c>
+      <c r="P19" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>639</v>
+      </c>
+      <c r="R19">
+        <v>2.6380041E-2</v>
+      </c>
+      <c r="S19">
+        <v>1.6837167E-2</v>
+      </c>
+      <c r="T19">
+        <v>0.834353083</v>
+      </c>
+      <c r="Y19">
+        <v>1460</v>
+      </c>
+      <c r="Z19">
+        <v>1108</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC19">
+        <v>1.9010397910000001</v>
+      </c>
+      <c r="AD19">
+        <v>0.14250325</v>
+      </c>
+      <c r="AE19">
+        <v>6.9029567500000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>145</v>
+      </c>
+      <c r="B20">
+        <v>31946</v>
+      </c>
+      <c r="E20" t="s">
+        <v>638</v>
+      </c>
+      <c r="F20" t="s">
+        <v>639</v>
+      </c>
+      <c r="G20">
+        <v>4.7046749999999998E-2</v>
+      </c>
+      <c r="H20">
+        <v>1.2442083E-2</v>
+      </c>
+      <c r="I20">
+        <v>1.2785131249999999</v>
+      </c>
+      <c r="L20">
+        <v>83</v>
+      </c>
+      <c r="M20">
+        <v>1772</v>
+      </c>
+      <c r="N20">
+        <v>87</v>
+      </c>
+      <c r="O20">
+        <v>437</v>
+      </c>
+      <c r="P20" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>639</v>
+      </c>
+      <c r="R20">
+        <v>1.7754499999999999E-2</v>
+      </c>
+      <c r="S20">
+        <v>1.4192209000000001E-2</v>
+      </c>
+      <c r="T20">
+        <v>0.89786449999999995</v>
+      </c>
+      <c r="Z20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC20">
+        <v>1.360954167</v>
+      </c>
+      <c r="AD20">
+        <v>1.9259083999999999E-2</v>
+      </c>
+      <c r="AE20">
+        <v>6.0306444170000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>146</v>
+      </c>
+      <c r="B21">
+        <v>32303</v>
+      </c>
+      <c r="E21" t="s">
+        <v>638</v>
+      </c>
+      <c r="F21" t="s">
+        <v>639</v>
+      </c>
+      <c r="G21">
+        <v>4.3649167000000003E-2</v>
+      </c>
+      <c r="H21">
+        <v>1.1217334000000001E-2</v>
+      </c>
+      <c r="I21">
+        <v>1.660987625</v>
+      </c>
+      <c r="L21">
+        <v>79</v>
+      </c>
+      <c r="M21">
+        <v>1791</v>
+      </c>
+      <c r="N21">
+        <v>87</v>
+      </c>
+      <c r="O21">
+        <v>437</v>
+      </c>
+      <c r="P21" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>639</v>
+      </c>
+      <c r="R21">
+        <v>1.898975E-2</v>
+      </c>
+      <c r="S21">
+        <v>1.1788834E-2</v>
+      </c>
+      <c r="T21">
+        <v>0.82053137499999995</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC21">
+        <v>1.409689875</v>
+      </c>
+      <c r="AD21">
+        <v>1.4225375E-2</v>
+      </c>
+      <c r="AE21">
+        <v>6.1729332919999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>145</v>
+      </c>
+      <c r="B22">
+        <v>32556</v>
+      </c>
+      <c r="E22" t="s">
+        <v>638</v>
+      </c>
+      <c r="F22" t="s">
+        <v>639</v>
+      </c>
+      <c r="G22">
+        <v>4.0089374999999997E-2</v>
+      </c>
+      <c r="H22">
+        <v>1.1471916E-2</v>
+      </c>
+      <c r="I22">
+        <v>1.580693125</v>
+      </c>
+      <c r="L22">
+        <v>97</v>
+      </c>
+      <c r="M22">
+        <v>1779</v>
+      </c>
+      <c r="N22">
+        <v>87</v>
+      </c>
+      <c r="O22">
+        <v>432</v>
+      </c>
+      <c r="P22" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>639</v>
+      </c>
+      <c r="R22">
+        <v>1.7281874999999999E-2</v>
+      </c>
+      <c r="S22">
+        <v>1.0896792000000001E-2</v>
+      </c>
+      <c r="T22">
+        <v>0.62807945799999998</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC22">
+        <v>1.3477914580000001</v>
+      </c>
+      <c r="AD22">
+        <v>1.1293666000000001E-2</v>
+      </c>
+      <c r="AE22">
+        <v>6.3103378750000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AA23" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC23">
+        <v>1.3321080830000001</v>
+      </c>
+      <c r="AD23">
+        <v>1.0731582999999999E-2</v>
+      </c>
+      <c r="AE23">
+        <v>6.4298470830000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f>AVERAGE(A18:A22)</f>
+        <v>146.80000000000001</v>
+      </c>
+      <c r="B24">
+        <f>AVERAGE(B18:B22)</f>
+        <v>32206.2</v>
+      </c>
+      <c r="G24">
+        <f>AVERAGE(G18:G22)</f>
+        <v>0.11393161659999999</v>
+      </c>
+      <c r="H24">
+        <f>AVERAGE(H18:H22)</f>
+        <v>4.0173424999999999E-2</v>
+      </c>
+      <c r="I24">
+        <f>AVERAGE(I18:I22)</f>
+        <v>1.3960747497999999</v>
+      </c>
+      <c r="L24">
+        <f>AVERAGE(L18:L22)</f>
+        <v>84.4</v>
+      </c>
+      <c r="M24">
+        <f>AVERAGE(M18:M22)</f>
+        <v>1765.8</v>
+      </c>
+      <c r="N24">
+        <f>AVERAGE(N18:N22)</f>
+        <v>86.6</v>
+      </c>
+      <c r="O24">
+        <f>AVERAGE(O18:O22)</f>
+        <v>434.8</v>
+      </c>
+      <c r="R24">
+        <f>AVERAGE(R18:R22)</f>
+        <v>8.4898899800000011E-2</v>
+      </c>
+      <c r="S24">
+        <f>AVERAGE(S18:S22)</f>
+        <v>3.9723875400000004E-2</v>
+      </c>
+      <c r="T24">
+        <f>AVERAGE(T18:T22)</f>
+        <v>0.83568441660000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AC25">
+        <f>AVERAGE(AC19:AC23)</f>
+        <v>1.4703166748000001</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" ref="AD25:AE25" si="1">AVERAGE(AD19:AD23)</f>
+        <v>3.9602591600000001E-2</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="1"/>
+        <v>6.3693438834000009</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="W28" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="W29" t="s">
+        <v>629</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="W30" t="s">
+        <v>630</v>
+      </c>
+      <c r="X30" t="s">
+        <v>631</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>631</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="Y31">
+        <v>1533</v>
+      </c>
+      <c r="Z31">
+        <v>1698</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC31">
+        <v>2.0023260839999999</v>
+      </c>
+      <c r="AD31">
+        <v>0.142380584</v>
+      </c>
+      <c r="AE31">
+        <v>8.1435879579999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="Y32">
+        <v>1634</v>
+      </c>
+      <c r="Z32">
+        <v>1697</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC32">
+        <v>1.3776858329999999</v>
+      </c>
+      <c r="AD32">
+        <v>1.7134416E-2</v>
+      </c>
+      <c r="AE32">
+        <v>7.7254482910000002</v>
+      </c>
+    </row>
+    <row r="33" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="Y33">
+        <v>1597</v>
+      </c>
+      <c r="Z33">
+        <v>1678</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC33">
+        <v>1.3806182499999999</v>
+      </c>
+      <c r="AD33">
+        <v>1.2453000000000001E-2</v>
+      </c>
+      <c r="AE33">
+        <v>7.7192425</v>
+      </c>
+    </row>
+    <row r="34" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="Z34">
+        <v>1.7</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC34">
+        <v>1.4006875000000001</v>
+      </c>
+      <c r="AD34">
+        <v>1.1336458000000001E-2</v>
+      </c>
+      <c r="AE34">
+        <v>7.3300331659999998</v>
+      </c>
+    </row>
+    <row r="35" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="AA35" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC35">
+        <v>1.3983008750000001</v>
+      </c>
+      <c r="AD35">
+        <v>1.1199166E-2</v>
+      </c>
+      <c r="AE35">
+        <v>7.5765903330000004</v>
+      </c>
+    </row>
+    <row r="37" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="AC37">
+        <f>AVERAGE(AC31:AC35)</f>
+        <v>1.5119237084000001</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" ref="AD37" si="2">AVERAGE(AD31:AD35)</f>
+        <v>3.8900724800000001E-2</v>
+      </c>
+      <c r="AE37">
+        <f>AVERAGE(AE31:AE35)</f>
+        <v>7.6989804496000005</v>
+      </c>
+    </row>
+    <row r="40" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="W40" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="41" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="Y41" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="42" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="Y42" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>631</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="Z43">
+        <v>2277</v>
+      </c>
+      <c r="AE43">
+        <v>9.6912108339999996</v>
+      </c>
+    </row>
+    <row r="44" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="Z44">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="W46" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="47" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="Y47" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="48" spans="23:31" x14ac:dyDescent="0.2">
+      <c r="Y48" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>631</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="26:31" x14ac:dyDescent="0.2">
+      <c r="Z49">
+        <v>3978</v>
+      </c>
+      <c r="AE49">
+        <v>11.906339209</v>
+      </c>
+    </row>
+    <row r="50" spans="26:31" x14ac:dyDescent="0.2">
+      <c r="Z50">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D6D80B-C6BF-434A-9FC3-76A2673518DE}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>630</v>
+      </c>
+      <c r="B2" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1207</v>
+      </c>
+      <c r="B3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1231</v>
+      </c>
+      <c r="B4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1218</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1222</v>
+      </c>
+      <c r="B6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1228</v>
+      </c>
+      <c r="B7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>AVERAGE(A3:A7)</f>
+        <v>1221.2</v>
+      </c>
+      <c r="B9">
+        <f>AVERAGE(B3:B7)</f>
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>